<commit_message>
Lista contactos Villanova correccion
</commit_message>
<xml_diff>
--- a/Villanova/listaContactos.xlsx
+++ b/Villanova/listaContactos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\WhatsAutoA\Villanova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64269F61-88BA-4502-893C-82148AE55143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F43F937-F834-4DB5-8B97-EB2E4BEE733F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,13 +43,6 @@
     <t>52_7751235490</t>
   </si>
   <si>
-    <t>⏳ ¡El Día del Padre está a la vuelta de la esquina! Aprovecha nuestra promoción especial y haz que este día sea verdaderamente memorable para papá. ¡Corre a tu Villanova más cercano y encuentra un dulce regalo para él! 🎁👨‍👧‍👦
-Consulta nuestra página web para conocer todas nuestras sucursales: https://villanova.com.mx/sucursales/</t>
-  </si>
-  <si>
-    <t>C:\Users\Administrator\Desktop\WhatsAutoA\Images\diapadre.png</t>
-  </si>
-  <si>
     <t>52_7711073537</t>
   </si>
   <si>
@@ -255,6 +248,14 @@
   </si>
   <si>
     <t>52_7712952307</t>
+  </si>
+  <si>
+    <t>C:\Users\Administrator\Desktop\WhatsAutoA\Images\explanada.png</t>
+  </si>
+  <si>
+    <t>¿Te gustaría que te consintamos con un helado?  🍦
+¡Ven a nuestra INAUGURACIÓN en Explanada Pachuca este 20 de junio a las 5:00pm! Será una tarde increíblemente cool y llena de sabor. 🍦🍨
+¡Te esperamos!</t>
   </si>
 </sst>
 </file>
@@ -627,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C76"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -646,783 +647,783 @@
     </row>
     <row r="2" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C55" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C57" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C59" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C60" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C65" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C66" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C67" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C68" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C70" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C72" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1430,10 +1431,10 @@
         <v>3</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C73" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1441,10 +1442,10 @@
         <v>4</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C74" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1452,10 +1453,10 @@
         <v>5</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C75" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1463,10 +1464,10 @@
         <v>6</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lista contactos Villanova correccion 2
</commit_message>
<xml_diff>
--- a/Villanova/listaContactos.xlsx
+++ b/Villanova/listaContactos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\WhatsAutoA\Villanova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F43F937-F834-4DB5-8B97-EB2E4BEE733F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5454F8E0-3BA7-4B5B-8CF3-FA6968ADC4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,12 +250,12 @@
     <t>52_7712952307</t>
   </si>
   <si>
-    <t>C:\Users\Administrator\Desktop\WhatsAutoA\Images\explanada.png</t>
-  </si>
-  <si>
     <t>¿Te gustaría que te consintamos con un helado?  🍦
 ¡Ven a nuestra INAUGURACIÓN en Explanada Pachuca este 20 de junio a las 5:00pm! Será una tarde increíblemente cool y llena de sabor. 🍦🍨
 ¡Te esperamos!</t>
+  </si>
+  <si>
+    <t>C:\Users\4to Creativo\OneDrive\Desktop\WhatsAutoA\Images\explanada.png</t>
   </si>
 </sst>
 </file>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B76"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -650,10 +650,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -661,10 +661,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -672,10 +672,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -683,10 +683,10 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -694,10 +694,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -705,10 +705,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -716,10 +716,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -727,10 +727,10 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -738,10 +738,10 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -749,10 +749,10 @@
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -760,10 +760,10 @@
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -771,10 +771,10 @@
         <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -782,10 +782,10 @@
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -793,10 +793,10 @@
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -804,10 +804,10 @@
         <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -815,10 +815,10 @@
         <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -826,10 +826,10 @@
         <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -837,10 +837,10 @@
         <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -848,10 +848,10 @@
         <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -859,10 +859,10 @@
         <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -870,10 +870,10 @@
         <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -881,10 +881,10 @@
         <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -892,10 +892,10 @@
         <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,10 +903,10 @@
         <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -914,10 +914,10 @@
         <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -925,10 +925,10 @@
         <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -936,10 +936,10 @@
         <v>33</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -947,10 +947,10 @@
         <v>34</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -958,10 +958,10 @@
         <v>35</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -969,10 +969,10 @@
         <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -980,10 +980,10 @@
         <v>37</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -991,10 +991,10 @@
         <v>38</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1002,10 +1002,10 @@
         <v>39</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1013,10 +1013,10 @@
         <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1024,10 +1024,10 @@
         <v>16</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1035,10 +1035,10 @@
         <v>41</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1046,10 +1046,10 @@
         <v>42</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1057,10 +1057,10 @@
         <v>42</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1068,10 +1068,10 @@
         <v>43</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1079,10 +1079,10 @@
         <v>44</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1090,10 +1090,10 @@
         <v>45</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1101,10 +1101,10 @@
         <v>46</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1112,10 +1112,10 @@
         <v>47</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1123,10 +1123,10 @@
         <v>48</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1134,10 +1134,10 @@
         <v>49</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1145,10 +1145,10 @@
         <v>50</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1156,10 +1156,10 @@
         <v>51</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C48" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1167,10 +1167,10 @@
         <v>52</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C49" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1178,10 +1178,10 @@
         <v>53</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C50" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1189,10 +1189,10 @@
         <v>54</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1200,10 +1200,10 @@
         <v>55</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1211,10 +1211,10 @@
         <v>56</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1222,10 +1222,10 @@
         <v>57</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C54" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1233,10 +1233,10 @@
         <v>58</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C55" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1244,10 +1244,10 @@
         <v>59</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C56" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1255,10 +1255,10 @@
         <v>60</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1266,10 +1266,10 @@
         <v>61</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1277,10 +1277,10 @@
         <v>62</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1288,10 +1288,10 @@
         <v>63</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1299,10 +1299,10 @@
         <v>64</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C61" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1310,10 +1310,10 @@
         <v>65</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C62" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1321,10 +1321,10 @@
         <v>66</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C63" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1332,10 +1332,10 @@
         <v>67</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1343,10 +1343,10 @@
         <v>68</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C65" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1354,10 +1354,10 @@
         <v>69</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C66" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1365,10 +1365,10 @@
         <v>70</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1376,10 +1376,10 @@
         <v>71</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C68" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1387,10 +1387,10 @@
         <v>72</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C69" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1398,10 +1398,10 @@
         <v>73</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C70" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1409,10 +1409,10 @@
         <v>74</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C71" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1420,10 +1420,10 @@
         <v>75</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C72" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1431,10 +1431,10 @@
         <v>3</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C73" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1442,10 +1442,10 @@
         <v>4</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C74" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1453,10 +1453,10 @@
         <v>5</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C75" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1464,10 +1464,10 @@
         <v>6</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>